<commit_message>
upload and read xls to s3
</commit_message>
<xml_diff>
--- a/assets/data/books.xlsx
+++ b/assets/data/books.xlsx
@@ -5,7 +5,7 @@
   <fileSharing readOnlyRecommended="0" userName="teisha"/>
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="2" xWindow="240" yWindow="60" windowWidth="0" windowHeight="0" tabRatio="500"/>
+    <workbookView activeTab="3" xWindow="240" yWindow="60" windowWidth="0" windowHeight="0" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Books" sheetId="1" r:id="rId4"/>
@@ -16,17 +16,17 @@
   <calcPr/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1581923393" val="973" rev="124" revOS="4" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1581923393" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1581923393" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1581923393"/>
+      <pm:revision xmlns:pm="smNativeData" day="1581998596" val="973" rev="124" revOS="4" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1581998596" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1581998596" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1581998596"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8635" uniqueCount="7441">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8636" uniqueCount="7441">
   <si>
     <t>asin</t>
   </si>
@@ -22925,7 +22925,7 @@
     <t>asin</t>
   </si>
   <si>
-    <t>purchase_date</t>
+    <t>date</t>
   </si>
   <si>
     <t>B00R1WA92O</t>
@@ -23402,7 +23402,7 @@
     <t>07-27-15</t>
   </si>
   <si>
-    <t>READ</t>
+    <t>LISTENED</t>
   </si>
 </sst>
 </file>
@@ -23427,7 +23427,7 @@
       <sz val="12"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1581923393" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1581998596" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="240" lang="default"/>
             <pm:cs face="Times New Roman" sz="240" lang="default"/>
             <pm:ea face="SimSun" sz="240" lang="default"/>
@@ -23442,7 +23442,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1581923393" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1581998596" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -23464,7 +23464,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1581923393" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1581998596" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -23486,7 +23486,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1581923393"/>
+          <pm:border xmlns:pm="smNativeData" id="1581998596"/>
         </ext>
       </extLst>
     </border>
@@ -23505,7 +23505,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1581923393"/>
+          <pm:border xmlns:pm="smNativeData" id="1581998596"/>
         </ext>
       </extLst>
     </border>
@@ -23522,7 +23522,7 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1581923393" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1581998596" count="1">
         <pm:charStyle name="Normal" fontId="0" Id="1"/>
       </pm:charStyles>
     </ext>
@@ -23788,8 +23788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O595"/>
   <sheetViews>
-    <sheetView view="normal" topLeftCell="E284" workbookViewId="0">
-      <selection activeCell="I57" sqref="I57:I305"/>
+    <sheetView view="normal" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.60"/>
@@ -46706,7 +46706,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1581923393" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1581998596" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -46715,16 +46715,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1581923393" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1581923393" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1581923393" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1581923393" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1581998596" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1581998596" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1581998596" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1581998596" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1581923393" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1581998596" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -46876,7 +46876,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1581923393" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1581998596" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -46885,16 +46885,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1581923393" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1581923393" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1581923393" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1581923393" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1581998596" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1581998596" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1581998596" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1581998596" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1581923393" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1581998596" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -46907,7 +46907,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C258"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="normal" zoomScale="90" workbookViewId="0">
+    <sheetView view="normal" zoomScale="90" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -49758,7 +49758,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1581923393" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1581998596" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -49767,16 +49767,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1581923393" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1581923393" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1581923393" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1581923393" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1581998596" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1581998596" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1581998596" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1581998596" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1581923393" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1581998596" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -49789,8 +49789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E595"/>
   <sheetViews>
-    <sheetView view="normal" topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" view="normal" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="16.60"/>
@@ -49800,7 +49800,7 @@
     <col min="4" max="4" width="11.721311" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>7280</v>
       </c>
@@ -49808,7 +49808,10 @@
         <v>7281</v>
       </c>
       <c r="C1" t="s">
-        <v>7266</v>
+        <v>7238</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7267</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -53708,7 +53711,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1581923393" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1581998596" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -53717,16 +53720,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1581923393" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1581923393" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1581923393" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1581923393" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1581998596" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1581998596" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1581998596" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1581998596" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1581923393" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1581998596" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>